<commit_message>
Updated Photo and Resume
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Desktop\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06098741-8007-4F59-89D2-2DC57CF854AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEEEA27-8558-4C91-AD04-9F0E9834FE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2024,7 +2024,9 @@
       <c r="M18" s="34">
         <v>84.15</v>
       </c>
-      <c r="N18" s="35"/>
+      <c r="N18" s="35">
+        <v>78.14</v>
+      </c>
       <c r="O18" s="34">
         <v>2022</v>
       </c>

</xml_diff>